<commit_message>
Publish December through February
</commit_message>
<xml_diff>
--- a/GB Accounts 2024-25/GB Accounts Company 2025-03-31 (Mar25) Excel 2007/Companysecretary.xlsx
+++ b/GB Accounts 2024-25/GB Accounts Company 2025-03-31 (Mar25) Excel 2007/Companysecretary.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony/projects/diy-accounting/GB Accounts 2024-25/GB Accounts Company 2025-03-31 (Mar25) Excel 2007/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1638A063-966C-1A4B-9EBB-8005AF788A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15192" windowHeight="9216" tabRatio="849"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11160" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boardmeeting" sheetId="5" r:id="rId1"/>
@@ -13,7 +19,17 @@
     <sheet name="DirectorsInterests" sheetId="3" r:id="rId4"/>
     <sheet name="Charges&amp;Debentures" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -143,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
@@ -157,10 +173,12 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -171,6 +189,7 @@
       <sz val="9"/>
       <color indexed="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -214,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -282,9 +301,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -308,9 +326,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -348,7 +366,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -420,7 +438,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -593,25 +611,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="24" customWidth="1"/>
-    <col min="2" max="3" width="9.109375" style="24"/>
-    <col min="4" max="4" width="12.5546875" style="24" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="29"/>
-    <col min="6" max="6" width="14.44140625" style="24" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" style="24"/>
+    <col min="4" max="4" width="12.5" style="24" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="28"/>
+    <col min="6" max="6" width="14.5" style="24" customWidth="1"/>
     <col min="7" max="7" width="1.6640625" style="24" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="24"/>
+    <col min="8" max="16384" width="9.1640625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -620,18 +638,18 @@
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="22"/>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="F2" s="25"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="22"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -640,7 +658,7 @@
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="22"/>
       <c r="B4" s="22" t="s">
         <v>35</v>
@@ -651,7 +669,7 @@
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -660,7 +678,7 @@
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="22"/>
       <c r="B6" s="22" t="s">
         <v>34</v>
@@ -673,18 +691,18 @@
       </c>
       <c r="G6" s="22"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="27"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="22"/>
-      <c r="B8" s="28" t="str">
+      <c r="B8" s="27" t="str">
         <f>IF(E8&gt;0,"UPDATE REGISTERMEMBERS"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -696,7 +714,7 @@
       </c>
       <c r="G8" s="22"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
@@ -705,7 +723,7 @@
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="22"/>
       <c r="B10" s="22" t="s">
         <v>33</v>
@@ -716,7 +734,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
     </row>
-    <row r="11" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -742,7 +760,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -750,17 +768,17 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="19.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" style="6" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="6"/>
+    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -780,7 +798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
@@ -788,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
@@ -810,7 +828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -818,22 +836,22 @@
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="14" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="6" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="6"/>
+    <col min="10" max="10" width="10.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -854,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="21" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="21" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -886,7 +904,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="34.200000000000003" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
@@ -903,7 +921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="34.200000000000003" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="D4" s="11" t="s">
         <v>17</v>
       </c>
@@ -934,7 +952,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -942,17 +960,17 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="23" style="6" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="6"/>
+    <col min="5" max="5" width="25.5" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -969,7 +987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="D2" s="6" t="s">
         <v>22</v>
       </c>
@@ -991,7 +1009,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -999,18 +1017,18 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="19" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="18" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" style="18" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="18" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="18" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" style="18" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="18"/>
+    <col min="7" max="16384" width="9.1640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>24</v>
       </c>

</xml_diff>